<commit_message>
replaced (A) and reloaded
</commit_message>
<xml_diff>
--- a/Reports Folder/Staff Performance Overview/Merged Reports SPO/merged_spo_08-04-23.xlsx
+++ b/Reports Folder/Staff Performance Overview/Merged Reports SPO/merged_spo_08-04-23.xlsx
@@ -497,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -728,10 +728,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -740,10 +740,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="G5" t="n">
-        <v>61.42</v>
+        <v>88.34</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -758,41 +758,41 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="M5" t="n">
-        <v>61.42</v>
+        <v>88.34</v>
       </c>
       <c r="N5" t="n">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="O5" t="n">
-        <v>61.42</v>
+        <v>44.17</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Brook Accomando (A)</t>
+          <t>Chrissy Cummings</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F6" t="n">
-        <v>25</v>
+        <v>1939.82</v>
       </c>
       <c r="G6" t="n">
-        <v>26.92</v>
+        <v>2090.52</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -807,41 +807,41 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>25</v>
+        <v>1939.82</v>
       </c>
       <c r="M6" t="n">
-        <v>26.92</v>
+        <v>2090.52</v>
       </c>
       <c r="N6" t="n">
-        <v>25</v>
+        <v>71.84518518518519</v>
       </c>
       <c r="O6" t="n">
-        <v>26.92</v>
+        <v>77.42666666666666</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Chrissy Cummings</t>
+          <t>Danielle Mai</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="F7" t="n">
-        <v>1939.82</v>
+        <v>491</v>
       </c>
       <c r="G7" t="n">
-        <v>2090.52</v>
+        <v>528.73</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -850,47 +850,47 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>5.38</v>
       </c>
       <c r="L7" t="n">
-        <v>1939.82</v>
+        <v>496</v>
       </c>
       <c r="M7" t="n">
-        <v>2090.52</v>
+        <v>534.11</v>
       </c>
       <c r="N7" t="n">
-        <v>71.84518518518519</v>
+        <v>82.66666666666667</v>
       </c>
       <c r="O7" t="n">
-        <v>77.42666666666666</v>
+        <v>89.01833333333333</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Danielle Mai</t>
+          <t>Gabriella Marquez</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8" t="n">
         <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>2.1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>491</v>
+        <v>177.3</v>
       </c>
       <c r="G8" t="n">
-        <v>528.73</v>
+        <v>190.97</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -899,47 +899,47 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>5.38</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>496</v>
+        <v>177.3</v>
       </c>
       <c r="M8" t="n">
-        <v>534.11</v>
+        <v>190.97</v>
       </c>
       <c r="N8" t="n">
-        <v>82.66666666666667</v>
+        <v>59.1</v>
       </c>
       <c r="O8" t="n">
-        <v>89.01833333333333</v>
+        <v>63.65666666666667</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Gabriella Marquez</t>
+          <t>Izzy Kruis</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="F9" t="n">
-        <v>127.3</v>
+        <v>2493</v>
       </c>
       <c r="G9" t="n">
-        <v>137.09</v>
+        <v>2686.23</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -954,41 +954,41 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>127.3</v>
+        <v>2493</v>
       </c>
       <c r="M9" t="n">
-        <v>137.09</v>
+        <v>2686.23</v>
       </c>
       <c r="N9" t="n">
-        <v>63.65</v>
+        <v>69.25</v>
       </c>
       <c r="O9" t="n">
-        <v>68.545</v>
+        <v>74.61750000000001</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Gabriella Marquez (A)</t>
+          <t>Jasmine Gomez</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="F10" t="n">
-        <v>50</v>
+        <v>1215.6</v>
       </c>
       <c r="G10" t="n">
-        <v>53.88</v>
+        <v>1309.02</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1003,41 +1003,41 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>50</v>
+        <v>1215.6</v>
       </c>
       <c r="M10" t="n">
-        <v>53.88</v>
+        <v>1309.02</v>
       </c>
       <c r="N10" t="n">
-        <v>50</v>
+        <v>63.97894736842105</v>
       </c>
       <c r="O10" t="n">
-        <v>53.88</v>
+        <v>68.8957894736842</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Izzy Kruis</t>
+          <t>Jasmine Saiz</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C11" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E11" t="n">
-        <v>2.4</v>
+        <v>2.45</v>
       </c>
       <c r="F11" t="n">
-        <v>2493</v>
+        <v>3598</v>
       </c>
       <c r="G11" t="n">
-        <v>2686.23</v>
+        <v>3876.94</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1052,41 +1052,41 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>2493</v>
+        <v>3598</v>
       </c>
       <c r="M11" t="n">
-        <v>2686.23</v>
+        <v>3876.94</v>
       </c>
       <c r="N11" t="n">
-        <v>69.25</v>
+        <v>74.95833333333333</v>
       </c>
       <c r="O11" t="n">
-        <v>74.61750000000001</v>
+        <v>80.76958333333333</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Jasmine Gomez</t>
+          <t xml:space="preserve">Justyne Martinez </t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C12" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E12" t="n">
-        <v>1.9</v>
+        <v>2.3</v>
       </c>
       <c r="F12" t="n">
-        <v>1215.6</v>
+        <v>1833</v>
       </c>
       <c r="G12" t="n">
-        <v>1309.02</v>
+        <v>1973.87</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1101,41 +1101,41 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>1215.6</v>
+        <v>1833</v>
       </c>
       <c r="M12" t="n">
-        <v>1309.02</v>
+        <v>1973.87</v>
       </c>
       <c r="N12" t="n">
-        <v>63.97894736842105</v>
+        <v>76.375</v>
       </c>
       <c r="O12" t="n">
-        <v>68.8957894736842</v>
+        <v>82.24458333333332</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jasmine Saiz</t>
+          <t>Karen Trevizo</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>2.45</v>
+        <v>2.1</v>
       </c>
       <c r="F13" t="n">
-        <v>3598</v>
+        <v>367</v>
       </c>
       <c r="G13" t="n">
-        <v>3876.94</v>
+        <v>395.42</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1150,41 +1150,41 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>3598</v>
+        <v>367</v>
       </c>
       <c r="M13" t="n">
-        <v>3876.94</v>
+        <v>395.42</v>
       </c>
       <c r="N13" t="n">
-        <v>74.95833333333333</v>
+        <v>61.16666666666666</v>
       </c>
       <c r="O13" t="n">
-        <v>80.76958333333333</v>
+        <v>65.90333333333334</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Justyne Martinez </t>
+          <t>Krisdee Martinez</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D14" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14" t="n">
-        <v>2.3</v>
+        <v>2.4</v>
       </c>
       <c r="F14" t="n">
-        <v>1833</v>
+        <v>2270</v>
       </c>
       <c r="G14" t="n">
-        <v>1973.87</v>
+        <v>2445.98</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1199,41 +1199,41 @@
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>1833</v>
+        <v>2270</v>
       </c>
       <c r="M14" t="n">
-        <v>1973.87</v>
+        <v>2445.98</v>
       </c>
       <c r="N14" t="n">
-        <v>76.375</v>
+        <v>66.76470588235294</v>
       </c>
       <c r="O14" t="n">
-        <v>82.24458333333332</v>
+        <v>71.94058823529411</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Karen Trevizo</t>
+          <t>Maggie  Farrell</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E15" t="n">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="F15" t="n">
-        <v>367</v>
+        <v>2170.8</v>
       </c>
       <c r="G15" t="n">
-        <v>395.42</v>
+        <v>2337.67</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1242,47 +1242,47 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>45.5</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="L15" t="n">
-        <v>367</v>
+        <v>2216.3</v>
       </c>
       <c r="M15" t="n">
-        <v>395.42</v>
+        <v>2386.67</v>
       </c>
       <c r="N15" t="n">
-        <v>61.16666666666666</v>
+        <v>71.49354838709678</v>
       </c>
       <c r="O15" t="n">
-        <v>65.90333333333334</v>
+        <v>76.98935483870967</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Krisdee Martinez</t>
+          <t>Makayla Baca</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C16" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D16" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E16" t="n">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="F16" t="n">
-        <v>2270</v>
+        <v>3581</v>
       </c>
       <c r="G16" t="n">
-        <v>2445.98</v>
+        <v>3856.23</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1291,47 +1291,47 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>50.07</v>
       </c>
       <c r="L16" t="n">
-        <v>2270</v>
+        <v>3627.5</v>
       </c>
       <c r="M16" t="n">
-        <v>2445.98</v>
+        <v>3906.3</v>
       </c>
       <c r="N16" t="n">
-        <v>66.76470588235294</v>
+        <v>82.44318181818181</v>
       </c>
       <c r="O16" t="n">
-        <v>71.94058823529411</v>
+        <v>88.77954545454546</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Maggie  Farrell</t>
+          <t>Matthew Young</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C17" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="F17" t="n">
-        <v>2170.8</v>
+        <v>1139</v>
       </c>
       <c r="G17" t="n">
-        <v>2337.67</v>
+        <v>1227.22</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1340,47 +1340,47 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>45.5</v>
+        <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>2216.3</v>
+        <v>1139</v>
       </c>
       <c r="M17" t="n">
-        <v>2386.67</v>
+        <v>1227.22</v>
       </c>
       <c r="N17" t="n">
-        <v>71.49354838709678</v>
+        <v>67</v>
       </c>
       <c r="O17" t="n">
-        <v>76.98935483870967</v>
+        <v>72.18941176470588</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Makayla Baca</t>
+          <t>Vy Torino</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C18" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D18" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E18" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="F18" t="n">
-        <v>3581</v>
+        <v>2807.5</v>
       </c>
       <c r="G18" t="n">
-        <v>3856.23</v>
+        <v>3023.3</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1389,119 +1389,21 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>46.5</v>
+        <v>25</v>
       </c>
       <c r="K18" t="n">
-        <v>50.07</v>
+        <v>26.92</v>
       </c>
       <c r="L18" t="n">
-        <v>3627.5</v>
+        <v>2832.5</v>
       </c>
       <c r="M18" t="n">
-        <v>3906.3</v>
+        <v>3050.22</v>
       </c>
       <c r="N18" t="n">
-        <v>82.44318181818181</v>
+        <v>76.55405405405405</v>
       </c>
       <c r="O18" t="n">
-        <v>88.77954545454546</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Matthew Young</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>17</v>
-      </c>
-      <c r="C19" t="n">
-        <v>16</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1139</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1227.22</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" t="n">
-        <v>1139</v>
-      </c>
-      <c r="M19" t="n">
-        <v>1227.22</v>
-      </c>
-      <c r="N19" t="n">
-        <v>67</v>
-      </c>
-      <c r="O19" t="n">
-        <v>72.18941176470588</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Vy Torino</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>37</v>
-      </c>
-      <c r="C20" t="n">
-        <v>11</v>
-      </c>
-      <c r="D20" t="n">
-        <v>17</v>
-      </c>
-      <c r="E20" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="F20" t="n">
-        <v>2807.5</v>
-      </c>
-      <c r="G20" t="n">
-        <v>3023.3</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="n">
-        <v>25</v>
-      </c>
-      <c r="K20" t="n">
-        <v>26.92</v>
-      </c>
-      <c r="L20" t="n">
-        <v>2832.5</v>
-      </c>
-      <c r="M20" t="n">
-        <v>3050.22</v>
-      </c>
-      <c r="N20" t="n">
-        <v>76.55405405405405</v>
-      </c>
-      <c r="O20" t="n">
         <v>82.43837837837837</v>
       </c>
     </row>

</xml_diff>